<commit_message>
fixed folder design and add js folder
</commit_message>
<xml_diff>
--- a/Example Dowland File/Transaction History.xlsx
+++ b/Example Dowland File/Transaction History.xlsx
@@ -203,7 +203,7 @@
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="17.55" customWidth="1"/>
-    <col min="3" max="3" width="16.200000000000003" customWidth="1"/>
+    <col min="3" max="3" width="17.55" customWidth="1"/>
     <col min="4" max="4" width="20.25" customWidth="1"/>
     <col min="5" max="5" width="25.650000000000002" customWidth="1"/>
   </cols>
@@ -253,17 +253,17 @@
       </c>
       <c t="inlineStr" r="C3">
         <is>
-          <t xml:space="preserve">Kaan Company</t>
+          <t xml:space="preserve">Selin Company</t>
         </is>
       </c>
       <c t="inlineStr" r="D3">
         <is>
-          <t xml:space="preserve">100.00₺</t>
+          <t xml:space="preserve">500.00₺</t>
         </is>
       </c>
       <c t="inlineStr" r="E3">
         <is>
-          <t xml:space="preserve">09-12-2023 16:21:48</t>
+          <t xml:space="preserve">13-12-2023 18:39:39</t>
         </is>
       </c>
     </row>
@@ -273,47 +273,22 @@
       </c>
       <c t="inlineStr" r="B4">
         <is>
-          <t xml:space="preserve">Kaan Company</t>
+          <t xml:space="preserve">Selin Company</t>
         </is>
       </c>
       <c t="inlineStr" r="C4">
         <is>
-          <t xml:space="preserve">Veli Company</t>
+          <t xml:space="preserve">Ahmet Company</t>
         </is>
       </c>
       <c t="inlineStr" r="D4">
         <is>
-          <t xml:space="preserve">100.00₺</t>
+          <t xml:space="preserve">200.00₺</t>
         </is>
       </c>
       <c t="inlineStr" r="E4">
         <is>
-          <t xml:space="preserve">09-12-2023 16:22:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="65">
-        <v>3</v>
-      </c>
-      <c t="inlineStr" r="B5">
-        <is>
-          <t xml:space="preserve">Selin Company</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C5">
-        <is>
-          <t xml:space="preserve">Kaan Company</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D5">
-        <is>
-          <t xml:space="preserve">150.00₺</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="E5">
-        <is>
-          <t xml:space="preserve">09-12-2023 16:24:18</t>
+          <t xml:space="preserve">13-12-2023 18:48:48</t>
         </is>
       </c>
     </row>

</xml_diff>